<commit_message>
Updated Script and Excel template
</commit_message>
<xml_diff>
--- a/TeamsUserList.xlsx
+++ b/TeamsUserList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armin/Powershell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8512897C-F0B6-0643-83F8-F2EBB7A68AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782A44A8-7AF7-5749-B235-34C8751D6543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="500" windowWidth="27280" windowHeight="16940" xr2:uid="{70D2856F-A8E4-8344-BDE3-5E5399A91EC4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Department A" sheetId="1" r:id="rId1"/>
+    <sheet name="Nuernberg" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="118">
   <si>
     <t>UPN</t>
   </si>
@@ -231,66 +231,6 @@
     <t>zh-HK</t>
   </si>
   <si>
-    <t>CP_DE_Default</t>
-  </si>
-  <si>
-    <t>DP_DE_Nuernberg</t>
-  </si>
-  <si>
-    <t>VRP_DE_International</t>
-  </si>
-  <si>
-    <t>MoH_DE</t>
-  </si>
-  <si>
-    <t>MoH_ES</t>
-  </si>
-  <si>
-    <t>MoH_CA</t>
-  </si>
-  <si>
-    <t>MoH_AU</t>
-  </si>
-  <si>
-    <t>MoH_NZ</t>
-  </si>
-  <si>
-    <t>MoH_TH</t>
-  </si>
-  <si>
-    <t>MoH_MY</t>
-  </si>
-  <si>
-    <t>VRP_DE_Internal</t>
-  </si>
-  <si>
-    <t>VRP_DE_National</t>
-  </si>
-  <si>
-    <t>VRP_DE_Premium</t>
-  </si>
-  <si>
-    <t>VRP_ES_Internal</t>
-  </si>
-  <si>
-    <t>VRP_ES_National</t>
-  </si>
-  <si>
-    <t>VRP_ES_International</t>
-  </si>
-  <si>
-    <t>VRP_ES_Premium</t>
-  </si>
-  <si>
-    <t>DP_DE_Sugenheim</t>
-  </si>
-  <si>
-    <t>CP_ES_Default</t>
-  </si>
-  <si>
-    <t>CP_CA_Default</t>
-  </si>
-  <si>
     <t>+499113965979</t>
   </si>
   <si>
@@ -301,6 +241,165 @@
   </si>
   <si>
     <t>+499113965978</t>
+  </si>
+  <si>
+    <t>VRP-DE-Internal</t>
+  </si>
+  <si>
+    <t>VRP-DE-National</t>
+  </si>
+  <si>
+    <t>CP-DE-Default</t>
+  </si>
+  <si>
+    <t>DP-DE-Nuernberg</t>
+  </si>
+  <si>
+    <t>MoH-DE</t>
+  </si>
+  <si>
+    <t>DP-DE-Sugenheim</t>
+  </si>
+  <si>
+    <t>MoH-ES</t>
+  </si>
+  <si>
+    <t>CP-CA-Default</t>
+  </si>
+  <si>
+    <t>VRP-DE-International</t>
+  </si>
+  <si>
+    <t>MoH-CA</t>
+  </si>
+  <si>
+    <t>VRP-DE-Premium</t>
+  </si>
+  <si>
+    <t>MoH-AU</t>
+  </si>
+  <si>
+    <t>VRP-ES-Internal</t>
+  </si>
+  <si>
+    <t>MoH-NZ</t>
+  </si>
+  <si>
+    <t>VRP-ES-National</t>
+  </si>
+  <si>
+    <t>MoH-TH</t>
+  </si>
+  <si>
+    <t>VRP-ES-International</t>
+  </si>
+  <si>
+    <t>MoH-MY</t>
+  </si>
+  <si>
+    <t>VRP-ES-Premium</t>
+  </si>
+  <si>
+    <t>DP-DE-Neumarkt</t>
+  </si>
+  <si>
+    <t>DP-DE-Hengersberg</t>
+  </si>
+  <si>
+    <t>DP-ES-Barcelona</t>
+  </si>
+  <si>
+    <t>DP-AU-Sydney</t>
+  </si>
+  <si>
+    <t>DP-NZ-Auckland</t>
+  </si>
+  <si>
+    <t>DP-CA-Ontario</t>
+  </si>
+  <si>
+    <t>DP-TH-Bangkok</t>
+  </si>
+  <si>
+    <t>DP-MY-Puchong</t>
+  </si>
+  <si>
+    <t>VRP-CA-Internal</t>
+  </si>
+  <si>
+    <t>VRP-CA-National</t>
+  </si>
+  <si>
+    <t>VRP-CA-International</t>
+  </si>
+  <si>
+    <t>VRP-CA-Premium</t>
+  </si>
+  <si>
+    <t>VRP-AU-Internal</t>
+  </si>
+  <si>
+    <t>VRP-AU-National</t>
+  </si>
+  <si>
+    <t>VRP-AU-International</t>
+  </si>
+  <si>
+    <t>VRP-AU-Premium</t>
+  </si>
+  <si>
+    <t>VRP-NZ-Internal</t>
+  </si>
+  <si>
+    <t>VRP-NZ-National</t>
+  </si>
+  <si>
+    <t>VRP-NZ-International</t>
+  </si>
+  <si>
+    <t>VRP-NZ-Premium</t>
+  </si>
+  <si>
+    <t>VRP-TH-Internal</t>
+  </si>
+  <si>
+    <t>VRP-TH-National</t>
+  </si>
+  <si>
+    <t>VRP-TH-International</t>
+  </si>
+  <si>
+    <t>VRP-TH-Premium</t>
+  </si>
+  <si>
+    <t>VRP-MY-Internal</t>
+  </si>
+  <si>
+    <t>VRP-MY-National</t>
+  </si>
+  <si>
+    <t>VRP-MY-International</t>
+  </si>
+  <si>
+    <t>VRP-MY-Premium</t>
+  </si>
+  <si>
+    <t>CP-DE-Attendant</t>
+  </si>
+  <si>
+    <t>CP-AU-Default</t>
+  </si>
+  <si>
+    <t>CP-NZ-Default</t>
+  </si>
+  <si>
+    <t>CP-TH-Default</t>
+  </si>
+  <si>
+    <t>CP-MY-Default</t>
+  </si>
+  <si>
+    <t>CP-DE-NM-Attendant</t>
   </si>
 </sst>
 </file>
@@ -352,13 +451,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -366,10 +463,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -388,8 +485,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72688DB4-A831-6543-8DCE-EB5D0FCF7ABC}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0">
   <autoFilter ref="A1:G3" xr:uid="{72688DB4-A831-6543-8DCE-EB5D0FCF7ABC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{74B90709-0BD2-8641-A5C1-71EBCAF25A29}" name="UPN" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{07D9CA50-7C1C-014B-B89A-C95CADCDF560}" name="Number" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{74B90709-0BD2-8641-A5C1-71EBCAF25A29}" name="UPN" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{07D9CA50-7C1C-014B-B89A-C95CADCDF560}" name="Number" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{AA4612B7-E4B9-A448-A4CD-6E8E98173CA9}" name="Calling Policy"/>
     <tableColumn id="4" xr3:uid="{93B1B584-C677-324A-9B0D-F3E2D426C2CA}" name="Dial Plan"/>
     <tableColumn id="5" xr3:uid="{F70133FD-DF20-5143-AFF9-83FE445C52B7}" name="Voice Routing Policy"/>
@@ -697,25 +794,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAD1D74-ED94-2E47-8E75-ABE3491F6314}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -738,66 +835,70 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>82</v>
+      <c r="A2" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>83</v>
+      <c r="A3" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+    </row>
   </sheetData>
+  <sheetProtection insertRows="0" sort="0"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{5212874D-5FB7-E147-9F8C-6F47D799EA52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{5212874D-5FB7-E147-9F8C-6F47D799EA52}">
       <formula1>VoiceMail</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{D7C6C8E4-2938-A843-8CA8-120D45436D0C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{D7C6C8E4-2938-A843-8CA8-120D45436D0C}">
       <formula1>CallHoldPolices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{B728CC8B-178B-2F4E-8C59-61D12706B232}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4" xr:uid="{B728CC8B-178B-2F4E-8C59-61D12706B232}">
       <formula1>VoiceRoutingPolicies</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{D5F23FBD-4A4B-2842-9A92-557AD0CC3159}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{D5F23FBD-4A4B-2842-9A92-557AD0CC3159}">
       <formula1>DialPlans</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{381EBE07-3955-0A46-90C8-D0FBCF8CBFC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4" xr:uid="{381EBE07-3955-0A46-90C8-D0FBCF8CBFC6}">
       <formula1>CallingPolicies</formula1>
     </dataValidation>
   </dataValidations>
@@ -816,7 +917,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,16 +931,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -847,16 +948,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -864,186 +965,285 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>95</v>
+      </c>
       <c r="E12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
       <c r="E13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
       <c r="E15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
       <c r="E16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
       <c r="E17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
       <c r="E18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
       <c r="E19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
       <c r="E20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
       <c r="E21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
       <c r="E22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
       <c r="E23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>107</v>
+      </c>
       <c r="E24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
       <c r="E25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>109</v>
+      </c>
       <c r="E26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
       <c r="E27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
       <c r="E28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>38</v>
       </c>
@@ -1159,6 +1359,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="IRFdD9Z5PQBFi0Ds4P3x+EMJ8wmG8gNQN9LHxtDhY4Nz8jyePmmdzrCwNLeFBOnD4z9l82R3dt9vG9UmopqRpQ==" saltValue="ROGG1S9hLnPEzCFMEwxbCA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replaced Script with Import-Excel
</commit_message>
<xml_diff>
--- a/TeamsUserList.xlsx
+++ b/TeamsUserList.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armin/Powershell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C2C680-E113-D141-B034-D198D994CC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD02A5C-CF37-FD41-B147-46F273D94988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="2040" windowWidth="27640" windowHeight="15440" xr2:uid="{70D2856F-A8E4-8344-BDE3-5E5399A91EC4}"/>
+    <workbookView xWindow="1160" yWindow="2040" windowWidth="27640" windowHeight="15440" activeTab="1" xr2:uid="{70D2856F-A8E4-8344-BDE3-5E5399A91EC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="4" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CallHoldPolices">Data!$D:$D</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
   <si>
     <t>UPN</t>
   </si>
@@ -400,13 +401,91 @@
   </si>
   <si>
     <t>Emergency Policiy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="36"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>INSTRUCTIONS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Fill out the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet with the configured policies in MS Teams Admin Center.
+2. Copy the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Template</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet give it a name
+3. Fill the newly created sheet with customer data
+4. Run the script </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run-TeamsUserList.ps1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -429,6 +508,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -444,7 +544,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -476,16 +576,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53BFF5D-3824-4144-A286-B6F51FBB5F93}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,6 +1141,376 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F8C299-83F3-764D-8403-CFDA96649481}">
+  <dimension ref="B2:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="10"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:M26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCE978-1EE6-6E41-A701-649B13FFD622}">
   <dimension ref="A1:H55"/>
   <sheetViews>

</xml_diff>

<commit_message>
Adding PAAccount Check and Test-Path function
</commit_message>
<xml_diff>
--- a/TeamsUserList.xlsx
+++ b/TeamsUserList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armin/Powershell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B2601B-6520-6A43-B63D-7582F88768F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8816D-E49B-1F44-9C36-17FD279790F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="2040" windowWidth="27640" windowHeight="15440" activeTab="2" xr2:uid="{70D2856F-A8E4-8344-BDE3-5E5399A91EC4}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>UPN</t>
   </si>
@@ -320,6 +320,27 @@
       </rPr>
       <t>Run-TeamsUserList.ps1</t>
     </r>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>Simultaneous</t>
+  </si>
+  <si>
+    <t>Forwarding Types</t>
+  </si>
+  <si>
+    <t>Forwarding Target Types</t>
+  </si>
+  <si>
+    <t>Voicemail</t>
+  </si>
+  <si>
+    <t>SingleTarget</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -501,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -534,6 +555,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7BCE978-1EE6-6E41-A701-649B13FFD622}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1369,9 +1391,11 @@
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1396,83 +1420,104 @@
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
       <c r="H4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D5" s="1"/>
       <c r="H5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D6" s="1"/>
       <c r="H6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D7" s="1"/>
       <c r="H7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D8" s="1"/>
       <c r="H8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H16" t="s">
         <v>21</v>
       </c>

</xml_diff>